<commit_message>
Deploying to gh-pages from  @ 15f4ee8bea82595b25ca403825491a82b358044a 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-4-3.xlsx
+++ b/assets/excel/2021_1-4-3.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6310A6-3064-4BEE-8EA8-C8FFD45BB6D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EE402B-8D85-4963-99F6-6F2058B6AF0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{DF92A720-80F4-4FDF-A1CB-99CD19EC0500}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
@@ -109,13 +106,97 @@
     <t>17</t>
   </si>
   <si>
-    <t>1) Aufgeführt sind die 20 größten Wanderungssalden im Jahr 2019 als darunter Positionen der in der Zeile Ingesamt augewiesenen Werte. "Staatenlos" sowie "ungeklärt und ohne Angabe" werden in Sonstige Ausprägungen geführt.</t>
-  </si>
-  <si>
     <t>Quelle: Wanderungsstatistik</t>
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Europa insgesamt            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Albanien                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Bulgarien                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Griechenland              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Italien                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kosovo                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Moldau, Republik          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Polen                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Rumänien                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Russische Föderation      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Serbien  (ab 2008)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Spanien                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Türkei                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ukraine                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EU Staaten                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afrika insgesamt            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amerika insgesamt           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asien insgesamt             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Afghanistan               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Indien                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Irak                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Iran,Islamische Republik  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kasachstan                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Libanon                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Syrien, Arabische Republik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australien und Ozeanien     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonstige Ziele              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insgesamt                   </t>
+  </si>
+  <si>
+    <t>1) Aufgeführt sind die 20 größten Wanderungssalden im Jahr 2020 als darunter Positionen der in der Zeile Ingesamt augewiesenen Werte. "Staatenlos" sowie "ungeklärt und ohne Angabe" werden in Sonstige Ausprägungen geführt.</t>
   </si>
 </sst>
 </file>
@@ -166,18 +247,12 @@
       <name val="NDSFrutiger 55 Roman"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -278,27 +353,6 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -314,21 +368,12 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -343,6 +388,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -358,166 +433,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="2020_1-4-3_Download"/>
-      <sheetName val="2020_1-4-3_Rohdaten"/>
-      <sheetName val="2020_1-4-3_CSV_Vorbereitung"/>
-      <sheetName val="2020_1-4-3_CSV_Export"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="3">
-          <cell r="B3" t="str">
-            <v xml:space="preserve">Europa insgesamt            </v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v xml:space="preserve">  Albanien                  </v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v xml:space="preserve">  Bulgarien                 </v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v xml:space="preserve">  Griechenland              </v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v xml:space="preserve">  Italien                   </v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8" t="str">
-            <v xml:space="preserve">  Kosovo                    </v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="str">
-            <v xml:space="preserve">  Moldau, Republik          </v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v xml:space="preserve">  Polen                     </v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v xml:space="preserve">  Rumänien                  </v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12" t="str">
-            <v xml:space="preserve">  Russische Föderation      </v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v xml:space="preserve">  Serbien  (ab 2008)        </v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14" t="str">
-            <v xml:space="preserve">  Spanien                   </v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15" t="str">
-            <v xml:space="preserve">  Türkei                    </v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16" t="str">
-            <v xml:space="preserve">  Ukraine                   </v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v xml:space="preserve"> EU Staaten                 </v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18" t="str">
-            <v xml:space="preserve">Afrika insgesamt            </v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19" t="str">
-            <v xml:space="preserve">Amerika insgesamt           </v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20" t="str">
-            <v xml:space="preserve">Asien insgesamt             </v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21" t="str">
-            <v xml:space="preserve">  Afghanistan               </v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22" t="str">
-            <v xml:space="preserve">  Indien                    </v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23" t="str">
-            <v xml:space="preserve">  Irak                      </v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24" t="str">
-            <v xml:space="preserve">  Iran,Islamische Republik  </v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25" t="str">
-            <v xml:space="preserve">  Kasachstan                </v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26" t="str">
-            <v xml:space="preserve">  Libanon                   </v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27" t="str">
-            <v xml:space="preserve">  Syrien, Arabische Republik</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28" t="str">
-            <v xml:space="preserve">Australien und Ozeanien     </v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29" t="str">
-            <v xml:space="preserve">Sonstige Ziele              </v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30" t="str">
-            <v xml:space="preserve">Insgesamt                   </v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -883,1735 +798,1707 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="9"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="26"/>
     </row>
     <row r="7" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="11">
+      <c r="B7" s="23"/>
+      <c r="C7" s="7">
         <v>2005</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="7">
         <v>2006</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="7">
         <v>2007</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="7">
         <v>2008</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="7">
         <v>2009</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="7">
         <v>2010</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="7">
         <v>2011</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="7">
         <v>2012</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="7">
         <v>2013</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="7">
         <v>2014</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="7">
         <v>2015</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="7">
         <v>2016</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="7">
         <v>2017</v>
       </c>
-      <c r="P7" s="11">
+      <c r="P7" s="7">
         <v>2018</v>
       </c>
-      <c r="Q7" s="11">
+      <c r="Q7" s="7">
         <v>2019</v>
       </c>
-      <c r="R7" s="12">
+      <c r="R7" s="8">
         <v>2020</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="14" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="15"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="28"/>
     </row>
     <row r="9" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="K9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="L9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="N9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="17" t="s">
+      <c r="O9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="17" t="s">
+      <c r="Q9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="R9" s="17" t="s">
+      <c r="R9" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B3</f>
-        <v xml:space="preserve">Europa insgesamt            </v>
-      </c>
-      <c r="C10" s="19">
+    <row r="10" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="30">
         <v>28436</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="30">
         <v>10389</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="30">
         <v>9514</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="30">
         <v>657</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="30">
         <v>2716</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="30">
         <v>9999</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="30">
         <v>17971</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="30">
         <v>21801</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="30">
         <v>24542</v>
       </c>
-      <c r="L10" s="19">
+      <c r="L10" s="30">
         <v>33237</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="30">
         <v>46652</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="30">
         <v>13142</v>
       </c>
-      <c r="O10" s="19">
+      <c r="O10" s="30">
         <v>28885</v>
       </c>
-      <c r="P10" s="19">
+      <c r="P10" s="30">
         <v>28790</v>
       </c>
-      <c r="Q10" s="19">
+      <c r="Q10" s="30">
         <v>22129</v>
       </c>
-      <c r="R10" s="19">
+      <c r="R10" s="30">
         <v>18765</v>
       </c>
     </row>
-    <row r="11" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B11" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B4</f>
-        <v xml:space="preserve">  Albanien                  </v>
-      </c>
-      <c r="C11" s="22">
+    <row r="11" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="31">
         <v>-12</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="31">
         <v>8</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="31">
         <v>6</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="31">
         <v>5</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="31">
         <v>-7</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="31">
         <v>-6</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="31">
         <v>23</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="31">
         <v>91</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="31">
         <v>287</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="31">
         <v>1687</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="31">
         <v>4365</v>
       </c>
-      <c r="N11" s="22">
+      <c r="N11" s="31">
         <v>-3085</v>
       </c>
-      <c r="O11" s="22">
+      <c r="O11" s="31">
         <v>-475</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="31">
         <v>360</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="Q11" s="31">
         <v>632</v>
       </c>
-      <c r="R11" s="22">
+      <c r="R11" s="31">
         <v>562</v>
       </c>
     </row>
-    <row r="12" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B12" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B5</f>
-        <v xml:space="preserve">  Bulgarien                 </v>
-      </c>
-      <c r="C12" s="22">
+    <row r="12" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="31">
         <v>10</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="31">
         <v>69</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="31">
         <v>553</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="31">
         <v>867</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="31">
         <v>499</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="31">
         <v>1045</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="31">
         <v>1193</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="31">
         <v>1439</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="31">
         <v>1385</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="31">
         <v>2957</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="31">
         <v>3977</v>
       </c>
-      <c r="N12" s="22">
+      <c r="N12" s="31">
         <v>2117</v>
       </c>
-      <c r="O12" s="22">
+      <c r="O12" s="31">
         <v>2734</v>
       </c>
-      <c r="P12" s="22">
+      <c r="P12" s="31">
         <v>2367</v>
       </c>
-      <c r="Q12" s="22">
+      <c r="Q12" s="31">
         <v>1600</v>
       </c>
-      <c r="R12" s="22">
+      <c r="R12" s="31">
         <v>2537</v>
       </c>
     </row>
-    <row r="13" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B13" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B6</f>
-        <v xml:space="preserve">  Griechenland              </v>
-      </c>
-      <c r="C13" s="22">
+    <row r="13" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="31">
         <v>-378</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="31">
         <v>-255</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="31">
         <v>-248</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="31">
         <v>-445</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="31">
         <v>-354</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="31">
         <v>59</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="31">
         <v>839</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="31">
         <v>1186</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="31">
         <v>1066</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="31">
         <v>773</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="31">
         <v>1079</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="31">
         <v>921</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="31">
         <v>818</v>
       </c>
-      <c r="P13" s="22">
+      <c r="P13" s="31">
         <v>865</v>
       </c>
-      <c r="Q13" s="22">
+      <c r="Q13" s="31">
         <v>517</v>
       </c>
-      <c r="R13" s="22">
+      <c r="R13" s="31">
         <v>632</v>
       </c>
     </row>
-    <row r="14" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B14" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B7</f>
-        <v xml:space="preserve">  Italien                   </v>
-      </c>
-      <c r="C14" s="22">
+    <row r="14" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="31">
         <v>-340</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="31">
         <v>-278</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="31">
         <v>-282</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="31">
         <v>-242</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="31">
         <v>-114</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="31">
         <v>381</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="31">
         <v>176</v>
       </c>
-      <c r="J14" s="22">
+      <c r="J14" s="31">
         <v>991</v>
       </c>
-      <c r="K14" s="22">
+      <c r="K14" s="31">
         <v>1581</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="31">
         <v>1659</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="31">
         <v>1845</v>
       </c>
-      <c r="N14" s="22">
+      <c r="N14" s="31">
         <v>1066</v>
       </c>
-      <c r="O14" s="22">
+      <c r="O14" s="31">
         <v>1303</v>
       </c>
-      <c r="P14" s="22">
+      <c r="P14" s="31">
         <v>1110</v>
       </c>
-      <c r="Q14" s="22">
+      <c r="Q14" s="31">
         <v>1103</v>
       </c>
-      <c r="R14" s="22">
+      <c r="R14" s="31">
         <v>837</v>
       </c>
     </row>
-    <row r="15" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B15" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B8</f>
-        <v xml:space="preserve">  Kosovo                    </v>
-      </c>
-      <c r="C15" s="22">
+    <row r="15" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B15" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="31">
         <v>0</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="31">
         <v>0</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="31">
         <v>0</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="31">
         <v>96</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="31">
         <v>212</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="31">
         <v>192</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="31">
         <v>240</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J15" s="31">
         <v>229</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="31">
         <v>460</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="31">
         <v>1350</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="31">
         <v>1736</v>
       </c>
-      <c r="N15" s="22">
+      <c r="N15" s="31">
         <v>-952</v>
       </c>
-      <c r="O15" s="22">
+      <c r="O15" s="31">
         <v>261</v>
       </c>
-      <c r="P15" s="22">
+      <c r="P15" s="31">
         <v>475</v>
       </c>
-      <c r="Q15" s="22">
+      <c r="Q15" s="31">
         <v>724</v>
       </c>
-      <c r="R15" s="22">
+      <c r="R15" s="31">
         <v>488</v>
       </c>
     </row>
-    <row r="16" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B16" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B9</f>
-        <v xml:space="preserve">  Moldau, Republik          </v>
-      </c>
-      <c r="C16" s="22">
+    <row r="16" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="31">
         <v>147</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="31">
         <v>35</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="31">
         <v>32</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="31">
         <v>36</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="31">
         <v>32</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="31">
         <v>56</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="31">
         <v>33</v>
       </c>
-      <c r="J16" s="22">
+      <c r="J16" s="31">
         <v>75</v>
       </c>
-      <c r="K16" s="22">
+      <c r="K16" s="31">
         <v>90</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="31">
         <v>302</v>
       </c>
-      <c r="M16" s="22">
+      <c r="M16" s="31">
         <v>496</v>
       </c>
-      <c r="N16" s="22">
+      <c r="N16" s="31">
         <v>645</v>
       </c>
-      <c r="O16" s="22">
+      <c r="O16" s="31">
         <v>948</v>
       </c>
-      <c r="P16" s="22">
+      <c r="P16" s="31">
         <v>1127</v>
       </c>
-      <c r="Q16" s="22">
+      <c r="Q16" s="31">
         <v>1414</v>
       </c>
-      <c r="R16" s="22">
+      <c r="R16" s="31">
         <v>1040</v>
       </c>
     </row>
-    <row r="17" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B17" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B10</f>
-        <v xml:space="preserve">  Polen                     </v>
-      </c>
-      <c r="C17" s="22">
+    <row r="17" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B17" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="31">
         <v>4937</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="31">
         <v>4548</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="31">
         <v>3865</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="31">
         <v>-508</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="31">
         <v>635</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="31">
         <v>2725</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="31">
         <v>7870</v>
       </c>
-      <c r="J17" s="22">
+      <c r="J17" s="31">
         <v>8059</v>
       </c>
-      <c r="K17" s="22">
+      <c r="K17" s="31">
         <v>7980</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="31">
         <v>8211</v>
       </c>
-      <c r="M17" s="22">
+      <c r="M17" s="31">
         <v>9466</v>
       </c>
-      <c r="N17" s="22">
+      <c r="N17" s="31">
         <v>3051</v>
       </c>
-      <c r="O17" s="22">
+      <c r="O17" s="31">
         <v>4250</v>
       </c>
-      <c r="P17" s="22">
+      <c r="P17" s="31">
         <v>2738</v>
       </c>
-      <c r="Q17" s="22">
+      <c r="Q17" s="31">
         <v>367</v>
       </c>
-      <c r="R17" s="22">
+      <c r="R17" s="31">
         <v>677</v>
       </c>
     </row>
-    <row r="18" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B18" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B11</f>
-        <v xml:space="preserve">  Rumänien                  </v>
-      </c>
-      <c r="C18" s="22">
+    <row r="18" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B18" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="31">
         <v>264</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="31">
         <v>271</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="31">
         <v>1288</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="31">
         <v>646</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="31">
         <v>916</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="31">
         <v>1860</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="31">
         <v>2693</v>
       </c>
-      <c r="J18" s="22">
+      <c r="J18" s="31">
         <v>2257</v>
       </c>
-      <c r="K18" s="22">
+      <c r="K18" s="31">
         <v>1978</v>
       </c>
-      <c r="L18" s="22">
+      <c r="L18" s="31">
         <v>5802</v>
       </c>
-      <c r="M18" s="22">
+      <c r="M18" s="31">
         <v>7216</v>
       </c>
-      <c r="N18" s="22">
+      <c r="N18" s="31">
         <v>5328</v>
       </c>
-      <c r="O18" s="22">
+      <c r="O18" s="31">
         <v>7347</v>
       </c>
-      <c r="P18" s="22">
+      <c r="P18" s="31">
         <v>6857</v>
       </c>
-      <c r="Q18" s="22">
+      <c r="Q18" s="31">
         <v>4306</v>
       </c>
-      <c r="R18" s="22">
+      <c r="R18" s="31">
         <v>4838</v>
       </c>
     </row>
-    <row r="19" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B19" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B12</f>
-        <v xml:space="preserve">  Russische Föderation      </v>
-      </c>
-      <c r="C19" s="22">
+    <row r="19" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="31">
         <v>21843</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="31">
         <v>5686</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="31">
         <v>3943</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="31">
         <v>2279</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G19" s="31">
         <v>2095</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="31">
         <v>1751</v>
       </c>
-      <c r="I19" s="22">
+      <c r="I19" s="31">
         <v>1590</v>
       </c>
-      <c r="J19" s="22">
+      <c r="J19" s="31">
         <v>1551</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="31">
         <v>2915</v>
       </c>
-      <c r="L19" s="22">
+      <c r="L19" s="31">
         <v>2928</v>
       </c>
-      <c r="M19" s="22">
+      <c r="M19" s="31">
         <v>3502</v>
       </c>
-      <c r="N19" s="22">
+      <c r="N19" s="31">
         <v>3933</v>
       </c>
-      <c r="O19" s="22">
+      <c r="O19" s="31">
         <v>3319</v>
       </c>
-      <c r="P19" s="22">
+      <c r="P19" s="31">
         <v>3913</v>
       </c>
-      <c r="Q19" s="22">
+      <c r="Q19" s="31">
         <v>3949</v>
       </c>
-      <c r="R19" s="22">
+      <c r="R19" s="31">
         <v>2202</v>
       </c>
     </row>
-    <row r="20" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B20" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B13</f>
-        <v xml:space="preserve">  Serbien  (ab 2008)        </v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="22">
+    <row r="20" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="31">
         <v>48</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="31">
         <v>-333</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="31">
         <v>318</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="31">
         <v>-87</v>
       </c>
-      <c r="J20" s="22">
+      <c r="J20" s="31">
         <v>213</v>
       </c>
-      <c r="K20" s="22">
+      <c r="K20" s="31">
         <v>791</v>
       </c>
-      <c r="L20" s="22">
+      <c r="L20" s="31">
         <v>1572</v>
       </c>
-      <c r="M20" s="22">
+      <c r="M20" s="31">
         <v>1150</v>
       </c>
-      <c r="N20" s="22">
+      <c r="N20" s="31">
         <v>-1552</v>
       </c>
-      <c r="O20" s="22">
+      <c r="O20" s="31">
         <v>234</v>
       </c>
-      <c r="P20" s="22">
+      <c r="P20" s="31">
         <v>541</v>
       </c>
-      <c r="Q20" s="22">
+      <c r="Q20" s="31">
         <v>490</v>
       </c>
-      <c r="R20" s="22">
+      <c r="R20" s="31">
         <v>489</v>
       </c>
     </row>
-    <row r="21" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B21" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B14</f>
-        <v xml:space="preserve">  Spanien                   </v>
-      </c>
-      <c r="C21" s="22">
+    <row r="21" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B21" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="31">
         <v>-304</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="31">
         <v>-419</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="31">
         <v>-198</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="31">
         <v>-361</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="31">
         <v>-16</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="31">
         <v>281</v>
       </c>
-      <c r="I21" s="22">
+      <c r="I21" s="31">
         <v>452</v>
       </c>
-      <c r="J21" s="22">
+      <c r="J21" s="31">
         <v>1107</v>
       </c>
-      <c r="K21" s="22">
+      <c r="K21" s="31">
         <v>1562</v>
       </c>
-      <c r="L21" s="22">
+      <c r="L21" s="31">
         <v>714</v>
       </c>
-      <c r="M21" s="22">
+      <c r="M21" s="31">
         <v>829</v>
       </c>
-      <c r="N21" s="22">
+      <c r="N21" s="31">
         <v>127</v>
       </c>
-      <c r="O21" s="22">
+      <c r="O21" s="31">
         <v>206</v>
       </c>
-      <c r="P21" s="22">
+      <c r="P21" s="31">
         <v>178</v>
       </c>
-      <c r="Q21" s="22">
+      <c r="Q21" s="31">
         <v>236</v>
       </c>
-      <c r="R21" s="22">
+      <c r="R21" s="31">
         <v>425</v>
       </c>
     </row>
-    <row r="22" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B22" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B15</f>
-        <v xml:space="preserve">  Türkei                    </v>
-      </c>
-      <c r="C22" s="22">
+    <row r="22" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B22" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="31">
         <v>31</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="31">
         <v>-306</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="31">
         <v>-203</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="31">
         <v>-554</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="31">
         <v>-440</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="31">
         <v>-206</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="31">
         <v>41</v>
       </c>
-      <c r="J22" s="22">
+      <c r="J22" s="31">
         <v>-140</v>
       </c>
-      <c r="K22" s="22">
+      <c r="K22" s="31">
         <v>-332</v>
       </c>
-      <c r="L22" s="22">
+      <c r="L22" s="31">
         <v>105</v>
       </c>
-      <c r="M22" s="22">
+      <c r="M22" s="31">
         <v>1240</v>
       </c>
-      <c r="N22" s="22">
+      <c r="N22" s="31">
         <v>1394</v>
       </c>
-      <c r="O22" s="22">
+      <c r="O22" s="31">
         <v>4136</v>
       </c>
-      <c r="P22" s="22">
+      <c r="P22" s="31">
         <v>3491</v>
       </c>
-      <c r="Q22" s="22">
+      <c r="Q22" s="31">
         <v>3628</v>
       </c>
-      <c r="R22" s="22">
+      <c r="R22" s="31">
         <v>1763</v>
       </c>
     </row>
-    <row r="23" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B23" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B16</f>
-        <v xml:space="preserve">  Ukraine                   </v>
-      </c>
-      <c r="C23" s="22">
+    <row r="23" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B23" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="31">
         <v>1514</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="31">
         <v>385</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="31">
         <v>411</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="31">
         <v>253</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="31">
         <v>388</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="31">
         <v>371</v>
       </c>
-      <c r="I23" s="22">
+      <c r="I23" s="31">
         <v>304</v>
       </c>
-      <c r="J23" s="22">
+      <c r="J23" s="31">
         <v>360</v>
       </c>
-      <c r="K23" s="22">
+      <c r="K23" s="31">
         <v>462</v>
       </c>
-      <c r="L23" s="22">
+      <c r="L23" s="31">
         <v>1002</v>
       </c>
-      <c r="M23" s="22">
+      <c r="M23" s="31">
         <v>1278</v>
       </c>
-      <c r="N23" s="22">
+      <c r="N23" s="31">
         <v>1185</v>
       </c>
-      <c r="O23" s="22">
+      <c r="O23" s="31">
         <v>1299</v>
       </c>
-      <c r="P23" s="22">
+      <c r="P23" s="31">
         <v>1433</v>
       </c>
-      <c r="Q23" s="22">
+      <c r="Q23" s="31">
         <v>1154</v>
       </c>
-      <c r="R23" s="22">
+      <c r="R23" s="31">
         <v>702</v>
       </c>
     </row>
-    <row r="24" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B24" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B17</f>
-        <v xml:space="preserve"> EU Staaten                 </v>
-      </c>
-      <c r="C24" s="22">
+    <row r="24" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B24" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="31">
         <v>6464</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="31">
         <v>5995</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="31">
         <v>6309</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F24" s="31">
         <v>607</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24" s="31">
         <v>1943</v>
       </c>
-      <c r="H24" s="22">
+      <c r="H24" s="31">
         <v>6335</v>
       </c>
-      <c r="I24" s="22">
+      <c r="I24" s="31">
         <v>13900</v>
       </c>
-      <c r="J24" s="22">
+      <c r="J24" s="31">
         <v>15364</v>
       </c>
-      <c r="K24" s="22">
+      <c r="K24" s="31">
         <v>15107</v>
       </c>
-      <c r="L24" s="22">
+      <c r="L24" s="31">
         <v>16581</v>
       </c>
-      <c r="M24" s="22">
+      <c r="M24" s="31">
         <v>20536</v>
       </c>
-      <c r="N24" s="22">
+      <c r="N24" s="31">
         <v>9569</v>
       </c>
-      <c r="O24" s="22">
+      <c r="O24" s="31">
         <v>13538</v>
       </c>
-      <c r="P24" s="22">
+      <c r="P24" s="31">
         <v>11661</v>
       </c>
-      <c r="Q24" s="22">
+      <c r="Q24" s="31">
         <v>5807</v>
       </c>
-      <c r="R24" s="22">
+      <c r="R24" s="31">
         <v>6782</v>
       </c>
     </row>
-    <row r="25" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B25" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B18</f>
-        <v xml:space="preserve">Afrika insgesamt            </v>
-      </c>
-      <c r="C25" s="22">
+    <row r="25" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="31">
         <v>361</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="31">
         <v>215</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="31">
         <v>404</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F25" s="31">
         <v>88</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G25" s="31">
         <v>384</v>
       </c>
-      <c r="H25" s="22">
+      <c r="H25" s="31">
         <v>649</v>
       </c>
-      <c r="I25" s="22">
+      <c r="I25" s="31">
         <v>838</v>
       </c>
-      <c r="J25" s="22">
+      <c r="J25" s="31">
         <v>1199</v>
       </c>
-      <c r="K25" s="22">
+      <c r="K25" s="31">
         <v>2863</v>
       </c>
-      <c r="L25" s="22">
+      <c r="L25" s="31">
         <v>4009</v>
       </c>
-      <c r="M25" s="22">
+      <c r="M25" s="31">
         <v>10488</v>
       </c>
-      <c r="N25" s="22">
+      <c r="N25" s="31">
         <v>2057</v>
       </c>
-      <c r="O25" s="22">
+      <c r="O25" s="31">
         <v>435</v>
       </c>
-      <c r="P25" s="22">
+      <c r="P25" s="31">
         <v>2810</v>
       </c>
-      <c r="Q25" s="22">
+      <c r="Q25" s="31">
         <v>3958</v>
       </c>
-      <c r="R25" s="22">
+      <c r="R25" s="31">
         <v>1873</v>
       </c>
     </row>
-    <row r="26" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B26" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B19</f>
-        <v xml:space="preserve">Amerika insgesamt           </v>
-      </c>
-      <c r="C26" s="22">
+    <row r="26" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="31">
         <v>-298</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="31">
         <v>-2</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="31">
         <v>-229</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="31">
         <v>-1035</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G26" s="31">
         <v>-170</v>
       </c>
-      <c r="H26" s="22">
+      <c r="H26" s="31">
         <v>42</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I26" s="31">
         <v>549</v>
       </c>
-      <c r="J26" s="22">
+      <c r="J26" s="31">
         <v>504</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K26" s="31">
         <v>213</v>
       </c>
-      <c r="L26" s="22">
+      <c r="L26" s="31">
         <v>402</v>
       </c>
-      <c r="M26" s="22">
+      <c r="M26" s="31">
         <v>630</v>
       </c>
-      <c r="N26" s="22">
+      <c r="N26" s="31">
         <v>507</v>
       </c>
-      <c r="O26" s="22">
+      <c r="O26" s="31">
         <v>1120</v>
       </c>
-      <c r="P26" s="22">
+      <c r="P26" s="31">
         <v>1453</v>
       </c>
-      <c r="Q26" s="22">
+      <c r="Q26" s="31">
         <v>1603</v>
       </c>
-      <c r="R26" s="22">
+      <c r="R26" s="31">
         <v>702</v>
       </c>
     </row>
-    <row r="27" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B27" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B20</f>
-        <v xml:space="preserve">Asien insgesamt             </v>
-      </c>
-      <c r="C27" s="22">
+    <row r="27" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B27" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="31">
         <v>13016</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="31">
         <v>2427</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="31">
         <v>2172</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F27" s="31">
         <v>1540</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G27" s="31">
         <v>4687</v>
       </c>
-      <c r="H27" s="22">
+      <c r="H27" s="31">
         <v>3888</v>
       </c>
-      <c r="I27" s="22">
+      <c r="I27" s="31">
         <v>4001</v>
       </c>
-      <c r="J27" s="22">
+      <c r="J27" s="31">
         <v>4526</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K27" s="31">
         <v>7392</v>
       </c>
-      <c r="L27" s="22">
+      <c r="L27" s="31">
         <v>16519</v>
       </c>
-      <c r="M27" s="22">
+      <c r="M27" s="31">
         <v>61462</v>
       </c>
-      <c r="N27" s="22">
+      <c r="N27" s="31">
         <v>41755</v>
       </c>
-      <c r="O27" s="22">
+      <c r="O27" s="31">
         <v>15521</v>
       </c>
-      <c r="P27" s="22">
+      <c r="P27" s="31">
         <v>13273</v>
       </c>
-      <c r="Q27" s="22">
+      <c r="Q27" s="31">
         <v>13061</v>
       </c>
-      <c r="R27" s="22">
+      <c r="R27" s="31">
         <v>8483</v>
       </c>
     </row>
-    <row r="28" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="18" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B21</f>
-        <v xml:space="preserve">  Afghanistan               </v>
-      </c>
-      <c r="C28" s="19">
+    <row r="28" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="30">
         <v>20</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="30">
         <v>-23</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="30">
         <v>4</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F28" s="30">
         <v>36</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="30">
         <v>243</v>
       </c>
-      <c r="H28" s="19">
+      <c r="H28" s="30">
         <v>512</v>
       </c>
-      <c r="I28" s="19">
+      <c r="I28" s="30">
         <v>538</v>
       </c>
-      <c r="J28" s="19">
+      <c r="J28" s="30">
         <v>433</v>
       </c>
-      <c r="K28" s="19">
+      <c r="K28" s="30">
         <v>489</v>
       </c>
-      <c r="L28" s="19">
+      <c r="L28" s="30">
         <v>703</v>
       </c>
-      <c r="M28" s="19">
+      <c r="M28" s="30">
         <v>8239</v>
       </c>
-      <c r="N28" s="19">
+      <c r="N28" s="30">
         <v>7203</v>
       </c>
-      <c r="O28" s="19">
+      <c r="O28" s="30">
         <v>415</v>
       </c>
-      <c r="P28" s="19">
+      <c r="P28" s="30">
         <v>418</v>
       </c>
-      <c r="Q28" s="19">
+      <c r="Q28" s="30">
         <v>363</v>
       </c>
-      <c r="R28" s="19">
+      <c r="R28" s="30">
         <v>713</v>
       </c>
     </row>
-    <row r="29" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="18" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B22</f>
-        <v xml:space="preserve">  Indien                    </v>
-      </c>
-      <c r="C29" s="19">
+    <row r="29" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="30">
         <v>77</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="30">
         <v>77</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E29" s="30">
         <v>101</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F29" s="30">
         <v>3</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="30">
         <v>97</v>
       </c>
-      <c r="H29" s="19">
+      <c r="H29" s="30">
         <v>243</v>
       </c>
-      <c r="I29" s="19">
+      <c r="I29" s="30">
         <v>162</v>
       </c>
-      <c r="J29" s="19">
+      <c r="J29" s="30">
         <v>213</v>
       </c>
-      <c r="K29" s="19">
+      <c r="K29" s="30">
         <v>270</v>
       </c>
-      <c r="L29" s="19">
+      <c r="L29" s="30">
         <v>331</v>
       </c>
-      <c r="M29" s="19">
+      <c r="M29" s="30">
         <v>303</v>
       </c>
-      <c r="N29" s="19">
+      <c r="N29" s="30">
         <v>419</v>
       </c>
-      <c r="O29" s="19">
+      <c r="O29" s="30">
         <v>605</v>
       </c>
-      <c r="P29" s="19">
+      <c r="P29" s="30">
         <v>801</v>
       </c>
-      <c r="Q29" s="19">
+      <c r="Q29" s="30">
         <v>1170</v>
       </c>
-      <c r="R29" s="19">
+      <c r="R29" s="30">
         <v>429</v>
       </c>
     </row>
-    <row r="30" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B30" s="18" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B23</f>
-        <v xml:space="preserve">  Irak                      </v>
-      </c>
-      <c r="C30" s="19">
+    <row r="30" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="30">
         <v>-48</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="30">
         <v>19</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="30">
         <v>176</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F30" s="30">
         <v>345</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="30">
         <v>2603</v>
       </c>
-      <c r="H30" s="19">
+      <c r="H30" s="30">
         <v>1176</v>
       </c>
-      <c r="I30" s="19">
+      <c r="I30" s="30">
         <v>525</v>
       </c>
-      <c r="J30" s="19">
+      <c r="J30" s="30">
         <v>244</v>
       </c>
-      <c r="K30" s="19">
+      <c r="K30" s="30">
         <v>366</v>
       </c>
-      <c r="L30" s="19">
+      <c r="L30" s="30">
         <v>969</v>
       </c>
-      <c r="M30" s="19">
+      <c r="M30" s="30">
         <v>10619</v>
       </c>
-      <c r="N30" s="19">
+      <c r="N30" s="30">
         <v>11434</v>
       </c>
-      <c r="O30" s="19">
+      <c r="O30" s="30">
         <v>3703</v>
       </c>
-      <c r="P30" s="19">
+      <c r="P30" s="30">
         <v>2179</v>
       </c>
-      <c r="Q30" s="19">
+      <c r="Q30" s="30">
         <v>1223</v>
       </c>
-      <c r="R30" s="19">
+      <c r="R30" s="30">
         <v>1092</v>
       </c>
     </row>
-    <row r="31" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B31" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B24</f>
-        <v xml:space="preserve">  Iran,Islamische Republik  </v>
-      </c>
-      <c r="C31" s="22">
+    <row r="31" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B31" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="31">
         <v>81</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="31">
         <v>37</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E31" s="31">
         <v>57</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="31">
         <v>29</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G31" s="31">
         <v>147</v>
       </c>
-      <c r="H31" s="22">
+      <c r="H31" s="31">
         <v>337</v>
       </c>
-      <c r="I31" s="22">
+      <c r="I31" s="31">
         <v>487</v>
       </c>
-      <c r="J31" s="22">
+      <c r="J31" s="31">
         <v>624</v>
       </c>
-      <c r="K31" s="22">
+      <c r="K31" s="31">
         <v>790</v>
       </c>
-      <c r="L31" s="22">
+      <c r="L31" s="31">
         <v>398</v>
       </c>
-      <c r="M31" s="22">
+      <c r="M31" s="31">
         <v>1830</v>
       </c>
-      <c r="N31" s="22">
+      <c r="N31" s="31">
         <v>2013</v>
       </c>
-      <c r="O31" s="22">
+      <c r="O31" s="31">
         <v>721</v>
       </c>
-      <c r="P31" s="22">
+      <c r="P31" s="31">
         <v>1388</v>
       </c>
-      <c r="Q31" s="22">
+      <c r="Q31" s="31">
         <v>1040</v>
       </c>
-      <c r="R31" s="22">
+      <c r="R31" s="31">
         <v>545</v>
       </c>
     </row>
-    <row r="32" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B32" s="18" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B25</f>
-        <v xml:space="preserve">  Kasachstan                </v>
-      </c>
-      <c r="C32" s="19">
+    <row r="32" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="30">
         <v>11234</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D32" s="30">
         <v>1693</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="30">
         <v>1320</v>
       </c>
-      <c r="F32" s="19">
+      <c r="F32" s="30">
         <v>962</v>
       </c>
-      <c r="G32" s="19">
+      <c r="G32" s="30">
         <v>834</v>
       </c>
-      <c r="H32" s="19">
+      <c r="H32" s="30">
         <v>483</v>
       </c>
-      <c r="I32" s="19">
+      <c r="I32" s="30">
         <v>559</v>
       </c>
-      <c r="J32" s="19">
+      <c r="J32" s="30">
         <v>430</v>
       </c>
-      <c r="K32" s="19">
+      <c r="K32" s="30">
         <v>809</v>
       </c>
-      <c r="L32" s="19">
+      <c r="L32" s="30">
         <v>2144</v>
       </c>
-      <c r="M32" s="19">
+      <c r="M32" s="30">
         <v>2022</v>
       </c>
-      <c r="N32" s="19">
+      <c r="N32" s="30">
         <v>2385</v>
       </c>
-      <c r="O32" s="19">
+      <c r="O32" s="30">
         <v>2653</v>
       </c>
-      <c r="P32" s="19">
+      <c r="P32" s="30">
         <v>2340</v>
       </c>
-      <c r="Q32" s="19">
+      <c r="Q32" s="30">
         <v>2584</v>
       </c>
-      <c r="R32" s="19">
+      <c r="R32" s="30">
         <v>1710</v>
       </c>
     </row>
-    <row r="33" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B33" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B26</f>
-        <v xml:space="preserve">  Libanon                   </v>
-      </c>
-      <c r="C33" s="22">
+    <row r="33" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B33" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="31">
         <v>23</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="31">
         <v>144</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33" s="31">
         <v>59</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="31">
         <v>87</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G33" s="31">
         <v>-44</v>
       </c>
-      <c r="H33" s="22">
+      <c r="H33" s="31">
         <v>54</v>
       </c>
-      <c r="I33" s="22">
+      <c r="I33" s="31">
         <v>42</v>
       </c>
-      <c r="J33" s="22">
+      <c r="J33" s="31">
         <v>88</v>
       </c>
-      <c r="K33" s="22">
+      <c r="K33" s="31">
         <v>179</v>
       </c>
-      <c r="L33" s="22">
+      <c r="L33" s="31">
         <v>562</v>
       </c>
-      <c r="M33" s="22">
+      <c r="M33" s="31">
         <v>1277</v>
       </c>
-      <c r="N33" s="22">
+      <c r="N33" s="31">
         <v>677</v>
       </c>
-      <c r="O33" s="22">
+      <c r="O33" s="31">
         <v>362</v>
       </c>
-      <c r="P33" s="22">
+      <c r="P33" s="31">
         <v>322</v>
       </c>
-      <c r="Q33" s="22">
+      <c r="Q33" s="31">
         <v>1069</v>
       </c>
-      <c r="R33" s="22">
+      <c r="R33" s="31">
         <v>511</v>
       </c>
     </row>
-    <row r="34" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B34" s="18" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B27</f>
-        <v xml:space="preserve">  Syrien, Arabische Republik</v>
-      </c>
-      <c r="C34" s="19">
+    <row r="34" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="30">
         <v>130</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D34" s="30">
         <v>58</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E34" s="30">
         <v>49</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F34" s="30">
         <v>62</v>
       </c>
-      <c r="G34" s="19">
+      <c r="G34" s="30">
         <v>189</v>
       </c>
-      <c r="H34" s="19">
+      <c r="H34" s="30">
         <v>302</v>
       </c>
-      <c r="I34" s="19">
+      <c r="I34" s="30">
         <v>610</v>
       </c>
-      <c r="J34" s="19">
+      <c r="J34" s="30">
         <v>860</v>
       </c>
-      <c r="K34" s="19">
+      <c r="K34" s="30">
         <v>2374</v>
       </c>
-      <c r="L34" s="19">
+      <c r="L34" s="30">
         <v>8965</v>
       </c>
-      <c r="M34" s="19">
+      <c r="M34" s="30">
         <v>32462</v>
       </c>
-      <c r="N34" s="19">
+      <c r="N34" s="30">
         <v>14970</v>
       </c>
-      <c r="O34" s="19">
+      <c r="O34" s="30">
         <v>4273</v>
       </c>
-      <c r="P34" s="19">
+      <c r="P34" s="30">
         <v>3042</v>
       </c>
-      <c r="Q34" s="19">
+      <c r="Q34" s="30">
         <v>2544</v>
       </c>
-      <c r="R34" s="19">
+      <c r="R34" s="30">
         <v>2368</v>
       </c>
     </row>
-    <row r="35" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B35" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B28</f>
-        <v xml:space="preserve">Australien und Ozeanien     </v>
-      </c>
-      <c r="C35" s="22">
+    <row r="35" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B35" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="31">
         <v>-124</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="31">
         <v>-107</v>
       </c>
-      <c r="E35" s="22">
+      <c r="E35" s="31">
         <v>-166</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="31">
         <v>-234</v>
       </c>
-      <c r="G35" s="22">
+      <c r="G35" s="31">
         <v>-164</v>
       </c>
-      <c r="H35" s="22">
+      <c r="H35" s="31">
         <v>-120</v>
       </c>
-      <c r="I35" s="22">
+      <c r="I35" s="31">
         <v>1</v>
       </c>
-      <c r="J35" s="22">
+      <c r="J35" s="31">
         <v>-23</v>
       </c>
-      <c r="K35" s="22">
+      <c r="K35" s="31">
         <v>-41</v>
       </c>
-      <c r="L35" s="22">
+      <c r="L35" s="31">
         <v>-72</v>
       </c>
-      <c r="M35" s="22">
+      <c r="M35" s="31">
         <v>-17</v>
       </c>
-      <c r="N35" s="22">
+      <c r="N35" s="31">
         <v>-71</v>
       </c>
-      <c r="O35" s="22">
+      <c r="O35" s="31">
         <v>-4</v>
       </c>
-      <c r="P35" s="22">
+      <c r="P35" s="31">
         <v>50</v>
       </c>
-      <c r="Q35" s="22">
+      <c r="Q35" s="31">
         <v>50</v>
       </c>
-      <c r="R35" s="22">
+      <c r="R35" s="31">
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B36" s="21" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B29</f>
-        <v xml:space="preserve">Sonstige Ziele              </v>
-      </c>
-      <c r="C36" s="22">
+    <row r="36" spans="2:18" s="14" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B36" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="31">
         <v>-874</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="31">
         <v>227</v>
       </c>
-      <c r="E36" s="22">
+      <c r="E36" s="31">
         <v>32</v>
       </c>
-      <c r="F36" s="22">
+      <c r="F36" s="31">
         <v>-66</v>
       </c>
-      <c r="G36" s="22">
+      <c r="G36" s="31">
         <v>190</v>
       </c>
-      <c r="H36" s="22">
+      <c r="H36" s="31">
         <v>0</v>
       </c>
-      <c r="I36" s="22">
+      <c r="I36" s="31">
         <v>310</v>
       </c>
-      <c r="J36" s="22">
+      <c r="J36" s="31">
         <v>-487</v>
       </c>
-      <c r="K36" s="22">
+      <c r="K36" s="31">
         <v>-34</v>
       </c>
-      <c r="L36" s="22">
+      <c r="L36" s="31">
         <v>-52</v>
       </c>
-      <c r="M36" s="22">
+      <c r="M36" s="31">
         <v>384</v>
       </c>
-      <c r="N36" s="22">
+      <c r="N36" s="31">
         <v>-19210</v>
       </c>
-      <c r="O36" s="22">
+      <c r="O36" s="31">
         <v>-7352</v>
       </c>
-      <c r="P36" s="22">
+      <c r="P36" s="31">
         <v>-1367</v>
       </c>
-      <c r="Q36" s="22">
+      <c r="Q36" s="31">
         <v>-2585</v>
       </c>
-      <c r="R36" s="22">
+      <c r="R36" s="31">
         <v>-2791</v>
       </c>
     </row>
-    <row r="37" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="18" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B30</f>
-        <v xml:space="preserve">Insgesamt                   </v>
-      </c>
-      <c r="C37" s="19">
+    <row r="37" spans="2:18" s="12" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B37" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="30">
         <v>40517</v>
       </c>
-      <c r="D37" s="19">
+      <c r="D37" s="30">
         <v>13149</v>
       </c>
-      <c r="E37" s="19">
+      <c r="E37" s="30">
         <v>11727</v>
       </c>
-      <c r="F37" s="19">
+      <c r="F37" s="30">
         <v>950</v>
       </c>
-      <c r="G37" s="19">
+      <c r="G37" s="30">
         <v>7643</v>
       </c>
-      <c r="H37" s="19">
+      <c r="H37" s="30">
         <v>14458</v>
       </c>
-      <c r="I37" s="19">
+      <c r="I37" s="30">
         <v>23670</v>
       </c>
-      <c r="J37" s="19">
+      <c r="J37" s="30">
         <v>27520</v>
       </c>
-      <c r="K37" s="19">
+      <c r="K37" s="30">
         <v>34935</v>
       </c>
-      <c r="L37" s="19">
+      <c r="L37" s="30">
         <v>54043</v>
       </c>
-      <c r="M37" s="19">
+      <c r="M37" s="30">
         <v>119599</v>
       </c>
-      <c r="N37" s="19">
+      <c r="N37" s="30">
         <v>38180</v>
       </c>
-      <c r="O37" s="19">
+      <c r="O37" s="30">
         <v>38605</v>
       </c>
-      <c r="P37" s="19">
+      <c r="P37" s="30">
         <v>45009</v>
       </c>
-      <c r="Q37" s="19">
+      <c r="Q37" s="30">
         <v>38216</v>
       </c>
-      <c r="R37" s="19">
+      <c r="R37" s="30">
         <v>27149</v>
       </c>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B38" s="24"/>
-    </row>
-    <row r="39" spans="2:18" s="26" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="25" t="s">
+      <c r="B38" s="15"/>
+    </row>
+    <row r="39" spans="2:18" s="16" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
+      <c r="Q39" s="17"/>
+    </row>
+    <row r="40" spans="2:18" s="16" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="18"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="17"/>
+    </row>
+    <row r="41" spans="2:18" s="16" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="25"/>
-      <c r="Q39" s="27"/>
-    </row>
-    <row r="40" spans="2:18" s="26" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D40" s="28"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="27"/>
-    </row>
-    <row r="41" spans="2:18" s="26" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="31"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="29"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="29"/>
-      <c r="N41" s="29"/>
-      <c r="O41" s="29"/>
-      <c r="P41" s="29"/>
-      <c r="Q41" s="27"/>
-    </row>
-    <row r="42" spans="2:18" s="26" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="27"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="17"/>
+    </row>
+    <row r="42" spans="2:18" s="16" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>